<commit_message>
I did a revision
</commit_message>
<xml_diff>
--- a/Codes in xcel/sample.xlsx
+++ b/Codes in xcel/sample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ll;l;klnnm,n,</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>;l;;l;</t>
+  </si>
+  <si>
+    <t>kkkmn</t>
   </si>
 </sst>
 </file>
@@ -356,27 +359,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>